<commit_message>
fix issue with ps plots
</commit_message>
<xml_diff>
--- a/app/data/smd.xlsx
+++ b/app/data/smd.xlsx
@@ -405,7 +405,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>arrhythmia_base</t>
+          <t>arrhythmia</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -425,7 +425,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>pacemaker_base</t>
+          <t>pacemaker</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -445,7 +445,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>hyperlipidemia_base</t>
+          <t>hyperlipidemia</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -465,7 +465,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>hypertension_base</t>
+          <t>hypertension</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -485,7 +485,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>depression_base</t>
+          <t>depression</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -505,7 +505,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>epilepsy_base</t>
+          <t>epilepsy</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -525,7 +525,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>cardio_base</t>
+          <t>cardio</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -545,7 +545,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>cvd_base</t>
+          <t>cvd</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ihd_base</t>
+          <t>ihd</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -585,7 +585,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>pvd_base</t>
+          <t>pvd</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>vhd_base</t>
+          <t>vhd</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -625,7 +625,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>hepatic_base</t>
+          <t>hepatic</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>acute_renal_base</t>
+          <t>acute_renal</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -665,7 +665,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>chronic_renal_base</t>
+          <t>chronic_renal</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>hypokalemia_base</t>
+          <t>hypokalemia</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -705,7 +705,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>hypocalcemia_base</t>
+          <t>hypocalcemia</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>hypomagnesemia_base</t>
+          <t>hypomagnesemia</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>stroke_base</t>
+          <t>stroke</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -765,7 +765,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>copd_base</t>
+          <t>copd</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -785,7 +785,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>mi_base</t>
+          <t>mi</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -805,7 +805,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>suicidal_base</t>
+          <t>suicidal</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>chf_base</t>
+          <t>chf</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -945,7 +945,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>arrhythmia_base</t>
+          <t>arrhythmia</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -965,7 +965,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>pacemaker_base</t>
+          <t>pacemaker</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>hyperlipidemia_base</t>
+          <t>hyperlipidemia</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>hypertension_base</t>
+          <t>hypertension</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1025,7 +1025,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>depression_base</t>
+          <t>depression</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>epilepsy_base</t>
+          <t>epilepsy</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>cardio_base</t>
+          <t>cardio</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>cvd_base</t>
+          <t>cvd</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ihd_base</t>
+          <t>ihd</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>pvd_base</t>
+          <t>pvd</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>vhd_base</t>
+          <t>vhd</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>hepatic_base</t>
+          <t>hepatic</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1185,7 +1185,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>acute_renal_base</t>
+          <t>acute_renal</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>chronic_renal_base</t>
+          <t>chronic_renal</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>hypokalemia_base</t>
+          <t>hypokalemia</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>hypocalcemia_base</t>
+          <t>hypocalcemia</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>hypomagnesemia_base</t>
+          <t>hypomagnesemia</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>stroke_base</t>
+          <t>stroke</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>copd_base</t>
+          <t>copd</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>mi_base</t>
+          <t>mi</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>suicidal_base</t>
+          <t>suicidal</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1365,7 +1365,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>chf_base</t>
+          <t>chf</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>arrhythmia_base</t>
+          <t>arrhythmia</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>pacemaker_base</t>
+          <t>pacemaker</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>hyperlipidemia_base</t>
+          <t>hyperlipidemia</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>hypertension_base</t>
+          <t>hypertension</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>depression_base</t>
+          <t>depression</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>epilepsy_base</t>
+          <t>epilepsy</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>cardio_base</t>
+          <t>cardio</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1625,7 +1625,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>cvd_base</t>
+          <t>cvd</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>ihd_base</t>
+          <t>ihd</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>pvd_base</t>
+          <t>pvd</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>vhd_base</t>
+          <t>vhd</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>hepatic_base</t>
+          <t>hepatic</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>acute_renal_base</t>
+          <t>acute_renal</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1745,7 +1745,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>chronic_renal_base</t>
+          <t>chronic_renal</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>hypokalemia_base</t>
+          <t>hypokalemia</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>hypocalcemia_base</t>
+          <t>hypocalcemia</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>hypomagnesemia_base</t>
+          <t>hypomagnesemia</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>stroke_base</t>
+          <t>stroke</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1845,7 +1845,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>copd_base</t>
+          <t>copd</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1865,7 +1865,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>mi_base</t>
+          <t>mi</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>suicidal_base</t>
+          <t>suicidal</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>chf_base</t>
+          <t>chf</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2025,7 +2025,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>arrhythmia_base</t>
+          <t>arrhythmia</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2045,7 +2045,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>pacemaker_base</t>
+          <t>pacemaker</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>hyperlipidemia_base</t>
+          <t>hyperlipidemia</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>hypertension_base</t>
+          <t>hypertension</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2105,7 +2105,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>depression_base</t>
+          <t>depression</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2125,7 +2125,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>epilepsy_base</t>
+          <t>epilepsy</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>cardio_base</t>
+          <t>cardio</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>cvd_base</t>
+          <t>cvd</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2185,7 +2185,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>ihd_base</t>
+          <t>ihd</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>pvd_base</t>
+          <t>pvd</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>vhd_base</t>
+          <t>vhd</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2245,7 +2245,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>hepatic_base</t>
+          <t>hepatic</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>acute_renal_base</t>
+          <t>acute_renal</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>chronic_renal_base</t>
+          <t>chronic_renal</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2305,7 +2305,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>hypokalemia_base</t>
+          <t>hypokalemia</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2325,7 +2325,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>hypocalcemia_base</t>
+          <t>hypocalcemia</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2345,7 +2345,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>hypomagnesemia_base</t>
+          <t>hypomagnesemia</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2365,7 +2365,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>stroke_base</t>
+          <t>stroke</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>copd_base</t>
+          <t>copd</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2405,7 +2405,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>mi_base</t>
+          <t>mi</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>suicidal_base</t>
+          <t>suicidal</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>chf_base</t>
+          <t>chf</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2565,7 +2565,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>arrhythmia_base</t>
+          <t>arrhythmia</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>pacemaker_base</t>
+          <t>pacemaker</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2605,7 +2605,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>hyperlipidemia_base</t>
+          <t>hyperlipidemia</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>hypertension_base</t>
+          <t>hypertension</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2645,7 +2645,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>depression_base</t>
+          <t>depression</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>epilepsy_base</t>
+          <t>epilepsy</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>cardio_base</t>
+          <t>cardio</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>cvd_base</t>
+          <t>cvd</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>ihd_base</t>
+          <t>ihd</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2745,7 +2745,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>pvd_base</t>
+          <t>pvd</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>vhd_base</t>
+          <t>vhd</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -2785,7 +2785,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>hepatic_base</t>
+          <t>hepatic</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2805,7 +2805,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>acute_renal_base</t>
+          <t>acute_renal</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>chronic_renal_base</t>
+          <t>chronic_renal</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>hypokalemia_base</t>
+          <t>hypokalemia</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>hypocalcemia_base</t>
+          <t>hypocalcemia</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>hypomagnesemia_base</t>
+          <t>hypomagnesemia</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2905,7 +2905,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>stroke_base</t>
+          <t>stroke</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>copd_base</t>
+          <t>copd</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>mi_base</t>
+          <t>mi</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2965,7 +2965,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>suicidal_base</t>
+          <t>suicidal</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>chf_base</t>
+          <t>chf</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">

</xml_diff>